<commit_message>
time updated to 20 sec
</commit_message>
<xml_diff>
--- a/TestOutput/TestExecutionLogs.xlsx
+++ b/TestOutput/TestExecutionLogs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="55">
   <si>
     <t>==============================</t>
   </si>
@@ -192,6 +192,15 @@
 Command: [a4c42a36dd7dbe71a5ddb413d2a09073, findElements {using=xpath, value=//h2[@class='line-1']}]
 Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 144.0.3719.92, fedcm:accounts: true, goog:processID: 19572, ms:edgeOptions: {debuggerAddress: localhost:60233}, msedge: {msedgedriverVersion: 144.0.3719.92 (8380d6794b22..., userDataDir: C:\Users\2457223\AppData\Lo...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:60233/devtoo..., se:cdpVersion: 144.0.3719.92, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
 Session ID: a4c42a36dd7dbe71a5ddb413d2a09073</t>
+  </si>
+  <si>
+    <t>Error during search: Expected condition failed: waiting for element found by By.xpath: //div[contains(@class,'c-omni-suggestion-item')]//div[contains(text(),'Bangalore')] to be clickable, but the element was not found: org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//div[contains(@class,'c-omni-suggestion-item')]//div[contains(text(),'Bangalore')]"}.
+(tried for 15 seconds with 500 milliseconds interval)
+Build info: version: '4.40.0', revision: 'b3333f1'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 142.0.7444.176, chrome: {chromedriverVersion: 142.0.7444.175 (302067f14a4..., userDataDir: C:\Users\2457382\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52484}, goog:processID: 14520, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52484/devtoo..., se:cdpVersion: 142.0.7444.176, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 9d4310f28ca2e78faf41ff59fa9589c0</t>
   </si>
 </sst>
 </file>
@@ -236,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A126"/>
+  <dimension ref="A1:A160"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -872,6 +881,176 @@
         <v>53</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -879,7 +1058,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1125,6 +1304,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1132,7 +1351,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1498,6 +1717,141 @@
         <v>0</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1505,7 +1859,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A62"/>
+  <dimension ref="A1:A83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1821,6 +2175,111 @@
         <v>0</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
name path changed as wait not working
</commit_message>
<xml_diff>
--- a/TestOutput/TestExecutionLogs.xlsx
+++ b/TestOutput/TestExecutionLogs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="58">
   <si>
     <t>==============================</t>
   </si>
@@ -201,6 +201,36 @@
 Driver info: org.openqa.selenium.chrome.ChromeDriver
 Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 142.0.7444.176, chrome: {chromedriverVersion: 142.0.7444.175 (302067f14a4..., userDataDir: C:\Users\2457382\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52484}, goog:processID: 14520, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52484/devtoo..., se:cdpVersion: 142.0.7444.176, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
 Session ID: 9d4310f28ca2e78faf41ff59fa9589c0</t>
+  </si>
+  <si>
+    <t>Error during search: Expected condition failed: waiting for element found by By.xpath: //div[contains(text(),'Bangalore')] to be clickable, but the element was not found: org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//div[contains(text(),'Bangalore')]"}.
+(tried for 15 seconds with 500 milliseconds interval)
+Build info: version: '4.40.0', revision: 'b3333f1'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 142.0.7444.176, chrome: {chromedriverVersion: 142.0.7444.175 (302067f14a4..., userDataDir: C:\Users\2457382\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58569}, goog:processID: 11444, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58569/devtoo..., se:cdpVersion: 142.0.7444.176, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 86d10fbe4c0ea41f2bc6d58ba35182d5</t>
+  </si>
+  <si>
+    <t>Error during search: invalid session id: session deleted as the browser has closed the connection
+from disconnected: not connected to DevTools
+  (Session info: chrome=142.0.7444.176)
+Build info: version: '4.40.0', revision: 'b3333f1'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [28dc2a14f3dabfc3d7ac1b4d2d4b0598, sendKeysToElement {id=f.0EC9F77330D5E8046A6531791E6535AA.d.18207EDF1F27767DC78E19B2085C4269.e.2, value=[Ljava.lang.CharSequence;@1934339}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 142.0.7444.176, chrome: {chromedriverVersion: 142.0.7444.175 (302067f14a4..., userDataDir: C:\Users\2457382\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:57189}, goog:processID: 3700, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:57189/devtoo..., se:cdpVersion: 142.0.7444.176, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Element: [[ChromeDriver: chrome on windows (28dc2a14f3dabfc3d7ac1b4d2d4b0598)] -&gt; xpath: //input[@placeholder='Search location']]
+Session ID: 28dc2a14f3dabfc3d7ac1b4d2d4b0598</t>
+  </si>
+  <si>
+    <t>Scrolling error: invalid session id
+Build info: version: '4.40.0', revision: 'b3333f1'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [28dc2a14f3dabfc3d7ac1b4d2d4b0598, executeScript {script=window.scrollBy(0, 1000), args=[]}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 142.0.7444.176, chrome: {chromedriverVersion: 142.0.7444.175 (302067f14a4..., userDataDir: C:\Users\2457382\AppData\Lo...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:57189}, goog:processID: 3700, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:57189/devtoo..., se:cdpVersion: 142.0.7444.176, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 28dc2a14f3dabfc3d7ac1b4d2d4b0598</t>
   </si>
 </sst>
 </file>
@@ -245,7 +275,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A160"/>
+  <dimension ref="A1:A204"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1051,6 +1081,226 @@
         <v>32</v>
       </c>
     </row>
+    <row r="161">
+      <c r="A161" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1058,7 +1308,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1344,6 +1594,56 @@
         <v>50</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1351,7 +1651,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A99"/>
+  <dimension ref="A1:A135"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1852,6 +2152,186 @@
         <v>17</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1859,7 +2339,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A83"/>
+  <dimension ref="A1:A104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2280,6 +2760,111 @@
         <v>8</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
again path changed ad in previous we have just removed visibility now actuall path changed
</commit_message>
<xml_diff>
--- a/TestOutput/TestExecutionLogs.xlsx
+++ b/TestOutput/TestExecutionLogs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="58">
   <si>
     <t>==============================</t>
   </si>
@@ -275,7 +275,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A204"/>
+  <dimension ref="A1:A221"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1301,6 +1301,91 @@
         <v>32</v>
       </c>
     </row>
+    <row r="205">
+      <c r="A205" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1308,7 +1393,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1644,6 +1729,31 @@
         <v>50</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1651,7 +1761,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A135"/>
+  <dimension ref="A1:A144"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2332,6 +2442,51 @@
         <v>17</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2339,7 +2494,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2865,6 +3020,41 @@
         <v>8</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>